<commit_message>
town and census block matchup update
</commit_message>
<xml_diff>
--- a/data/data_tracking.xlsx
+++ b/data/data_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dasha\Desktop\insight_project\biobot_insight_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DCE11E-3DF1-418E-9E5E-F67F80E82790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C12E90B-20DB-45DD-AA27-C8846DC611A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1610" yWindow="0" windowWidth="22120" windowHeight="13800" activeTab="1" xr2:uid="{6294C74B-E0C9-44A1-81AA-DD5ED14ACE10}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
   <si>
     <t>File name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>What it is</t>
   </si>
   <si>
-    <t>Medicare Part D Opioid Prescriber Summary File 2017</t>
-  </si>
-  <si>
     <t>Dataset summary</t>
   </si>
   <si>
@@ -59,15 +56,6 @@
     <t>data.cms.gov (CMS)</t>
   </si>
   <si>
-    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2017</t>
-  </si>
-  <si>
-    <t>Medicare Part D Opioid Prescriber Summary File 2016</t>
-  </si>
-  <si>
-    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2016</t>
-  </si>
-  <si>
     <t>https://data.cms.gov/Medicare-Part-D/Medicare-Part-D-Opioid-Prescriber-Summary-File-201/6wg9-kwip</t>
   </si>
   <si>
@@ -77,42 +65,24 @@
     <t>opioid prescription data summarized by provider (2016) summarized at "opioid"</t>
   </si>
   <si>
-    <t>Medicare Part D Opioid Prescriber Summary File 2015</t>
-  </si>
-  <si>
     <t>https://data.cms.gov/Medicare-Part-D/Medicare-Part-D-Opioid-Prescriber-Summary-File-201/6i2k-7h8p</t>
   </si>
   <si>
     <t>opioid prescription data summarized by provider (2015) summarized at "opioid"</t>
   </si>
   <si>
-    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2015</t>
-  </si>
-  <si>
-    <t>Medicare Part D Opioid Prescriber Summary File 2014</t>
-  </si>
-  <si>
     <t>https://data.cms.gov/Medicare-Part-D/Medicare-Part-D-Opioid-Prescriber-Summary-File-201/e4ka-3ncx</t>
   </si>
   <si>
     <t>opioid prescription data summarized by provider (2014) summarized at "opioid"</t>
   </si>
   <si>
-    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2014</t>
-  </si>
-  <si>
-    <t>Medicare Part D Opioid Prescriber Summary File 2013</t>
-  </si>
-  <si>
     <t>https://data.cms.gov/Medicare-Part-D/Medicare-Part-D-Opioid-Prescriber-Summary-File-201/yb2j-f3fp</t>
   </si>
   <si>
     <t>opioid prescription data summarized by provider (2013) summarized at "opioid"</t>
   </si>
   <si>
-    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2013</t>
-  </si>
-  <si>
     <t>CDC_Oral_Morphine_Milligram_Equivalents_Sept_2018</t>
   </si>
   <si>
@@ -312,6 +282,42 @@
   </si>
   <si>
     <t>Not used further because of grouping method of overdose death counts</t>
+  </si>
+  <si>
+    <t>raw_data/medicare_prescription_all_drugs/</t>
+  </si>
+  <si>
+    <t>raw_data/medicare_prescription_opioids/</t>
+  </si>
+  <si>
+    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2013.csv</t>
+  </si>
+  <si>
+    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2014.csv</t>
+  </si>
+  <si>
+    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2015.csv</t>
+  </si>
+  <si>
+    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2016.csv</t>
+  </si>
+  <si>
+    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2017.csv</t>
+  </si>
+  <si>
+    <t>Data on opioid prescription rate by prescriber with associated zip code. Used to estimate opioid pill availability per town</t>
+  </si>
+  <si>
+    <t>Medicare_Part_D_Opioid_Prescribing_Mapping_Tool_Methodology</t>
+  </si>
+  <si>
+    <t>dataset summary and codebook from cms</t>
+  </si>
+  <si>
+    <t>raw_data/other_not_used/</t>
+  </si>
+  <si>
+    <t>raw_data/shapefiles_and_geography_related/</t>
   </si>
 </sst>
 </file>
@@ -684,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891DE753-94C5-49D5-A840-92C5F085CC82}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,7 +705,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -716,126 +722,41 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -845,10 +766,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346E222B-442B-4376-8D3F-E3761B1F991A}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -860,7 +781,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -868,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -877,112 +798,112 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1">
         <v>43723</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1">
         <v>43723</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>43723</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1">
         <v>43723</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1">
         <v>43723</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -990,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -999,58 +920,58 @@
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1">
         <v>43721</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1">
         <v>43721</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1058,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
@@ -1067,101 +988,314 @@
         <v>2</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1">
         <v>43720</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E19" s="1">
         <v>43723</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E20" s="1">
         <v>43723</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E21" s="1">
         <v>43723</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="1">
+        <v>43719</v>
+      </c>
+      <c r="F33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{A06239DA-1EF7-48F0-8B85-18B252279A34}"/>
     <hyperlink ref="D18" r:id="rId2" xr:uid="{57B83395-7527-4B74-A1DA-E565991406F3}"/>
+    <hyperlink ref="D33" r:id="rId3" xr:uid="{2958F1B8-0368-4195-8497-5925E3429781}"/>
+    <hyperlink ref="D34" r:id="rId4" xr:uid="{8BD99E14-70C7-4D70-A35F-8785C13C4DFA}"/>
+    <hyperlink ref="D35" r:id="rId5" xr:uid="{DF933CB7-EB9F-4605-A6F1-4340BAB67BCD}"/>
+    <hyperlink ref="D36" r:id="rId6" xr:uid="{6B7D5CBE-6D80-43E9-8D1F-F409047BFB63}"/>
+    <hyperlink ref="D37" r:id="rId7" xr:uid="{795FA866-B3AE-49B1-B806-F6A0B9BFE0D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1183,7 +1317,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1191,56 +1325,56 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notebook3 (census block and town match) update wrap up
Reran the matches - result was the same as what I had used down the line in other notebooks, but now the code here is a lot cleaner. Updated the number of towns where there was a mismatch in population after merging
</commit_message>
<xml_diff>
--- a/data/data_tracking.xlsx
+++ b/data/data_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dasha\Desktop\insight_project\biobot_insight_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C12E90B-20DB-45DD-AA27-C8846DC611A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA363823-BD2B-4332-B231-D754BD6EACEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1610" yWindow="0" windowWidth="22120" windowHeight="13800" activeTab="1" xr2:uid="{6294C74B-E0C9-44A1-81AA-DD5ED14ACE10}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="104">
   <si>
     <t>File name</t>
   </si>
@@ -318,6 +318,33 @@
   </si>
   <si>
     <t>raw_data/shapefiles_and_geography_related/</t>
+  </si>
+  <si>
+    <t>CENSUS2010_BLK_BG_TRCT_SHP/</t>
+  </si>
+  <si>
+    <t>Folder with 2010 MA census block shapefiles</t>
+  </si>
+  <si>
+    <t>Mass.gov</t>
+  </si>
+  <si>
+    <t>Used to merge census blocks with towns (assumption that 2010 census blocks are the same as ACS blocks - GEOID10 did match up)</t>
+  </si>
+  <si>
+    <t>https://docs.digital.mass.gov/dataset/massgis-data-datalayers-2010-us-census</t>
+  </si>
+  <si>
+    <t>townssurvey_shp/</t>
+  </si>
+  <si>
+    <t>Folder with MA town survey shapefiles (state of MA divided up into 351 municipalities/towns/cities)</t>
+  </si>
+  <si>
+    <t>Used to merge census blocks with towns</t>
+  </si>
+  <si>
+    <t>https://docs.digital.mass.gov/dataset/massgis-data-community-boundaries-towns-survey-points</t>
   </si>
 </sst>
 </file>
@@ -766,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346E222B-442B-4376-8D3F-E3761B1F991A}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1282,6 +1309,46 @@
       </c>
       <c r="G47" s="3" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="1">
+        <v>43723</v>
+      </c>
+      <c r="F48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="1">
+        <v>43724</v>
+      </c>
+      <c r="F49" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notebook error cleanup, figure modification, data tracking update
</commit_message>
<xml_diff>
--- a/data/data_tracking.xlsx
+++ b/data/data_tracking.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dasha\Desktop\insight_project\biobot_insight_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA363823-BD2B-4332-B231-D754BD6EACEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DF5AC-4765-47D1-9EE5-5F0E15648AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1610" yWindow="0" windowWidth="22120" windowHeight="13800" activeTab="1" xr2:uid="{6294C74B-E0C9-44A1-81AA-DD5ED14ACE10}"/>
+    <workbookView xWindow="1830" yWindow="0" windowWidth="22120" windowHeight="13800" activeTab="1" xr2:uid="{6294C74B-E0C9-44A1-81AA-DD5ED14ACE10}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="raw_data" sheetId="5" r:id="rId2"/>
-    <sheet name="tidy_data" sheetId="6" r:id="rId3"/>
+    <sheet name="raw_data" sheetId="5" r:id="rId1"/>
+    <sheet name="tidy_data" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="172">
   <si>
     <t>File name</t>
   </si>
@@ -44,9 +43,6 @@
     <t>Url</t>
   </si>
   <si>
-    <t>What it is</t>
-  </si>
-  <si>
     <t>Dataset summary</t>
   </si>
   <si>
@@ -83,39 +79,6 @@
     <t>opioid prescription data summarized by provider (2013) summarized at "opioid"</t>
   </si>
   <si>
-    <t>CDC_Oral_Morphine_Milligram_Equivalents_Sept_2018</t>
-  </si>
-  <si>
-    <t>Analyzing Prescription Data and Morphine Milligram Equivalents (MME)</t>
-  </si>
-  <si>
-    <t>Data files of select prescription medications, including opioids with estimated oral morphine milligram equivalent (MME) conversion factors, 2018 version.</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov/drugoverdose/resources/data.html</t>
-  </si>
-  <si>
-    <t>cdc</t>
-  </si>
-  <si>
-    <t>https://www.washingtonpost.com/graphics/2019/investigations/dea-pain-pill-database/#download-resources</t>
-  </si>
-  <si>
-    <t>WaPo DEA Pill tracking MA data</t>
-  </si>
-  <si>
-    <t>arcos-ma-statewide-itemized.tsv</t>
-  </si>
-  <si>
-    <t>WaPo/CDC</t>
-  </si>
-  <si>
-    <t>https://www.mass.gov/lists/substance-abuse-treatment-admissions-statistics</t>
-  </si>
-  <si>
-    <t>MA substance abuse data</t>
-  </si>
-  <si>
     <t>City Health Dashboard</t>
   </si>
   <si>
@@ -345,6 +308,246 @@
   </si>
   <si>
     <t>https://docs.digital.mass.gov/dataset/massgis-data-community-boundaries-towns-survey-points</t>
+  </si>
+  <si>
+    <t>Medicare Part D all drug prescription claims by prescriber (Year 2013)</t>
+  </si>
+  <si>
+    <t>Medicare Part D all drug prescription claims by prescriber (Year 2014)</t>
+  </si>
+  <si>
+    <t>Medicare Part D all drug prescription claims by prescriber (Year 2015)</t>
+  </si>
+  <si>
+    <t>Medicare Part D all drug prescription claims by prescriber (Year 2016)</t>
+  </si>
+  <si>
+    <t>Medicare Part D all drug prescription claims by prescriber (Year 2017)</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>https://www.cms.gov/Research-Statistics-Data-and-Systems/Statistics-Trends-and-Reports/Medicare-Provider-Charge-Data/PartD2017</t>
+  </si>
+  <si>
+    <t>https://www.cms.gov/Research-Statistics-Data-and-Systems/Statistics-Trends-and-Reports/Medicare-Provider-Charge-Data/PartD2016</t>
+  </si>
+  <si>
+    <t>https://www.cms.gov/Research-Statistics-Data-and-Systems/Statistics-Trends-and-Reports/Medicare-Provider-Charge-Data/PartD2015</t>
+  </si>
+  <si>
+    <t>https://www.cms.gov/Research-Statistics-Data-and-Systems/Statistics-Trends-and-Reports/Medicare-Provider-Charge-Data/PartD2014</t>
+  </si>
+  <si>
+    <t>https://www.cms.gov/Research-Statistics-Data-and-Systems/Statistics-Trends-and-Reports/Medicare-Provider-Charge-Data/PartD2013</t>
+  </si>
+  <si>
+    <t>These files are tab delimited; very large (2.7-3 GB each)</t>
+  </si>
+  <si>
+    <t>Source of benzodiazepine claims; Extracted in notebook 5</t>
+  </si>
+  <si>
+    <t>Prescriber_Methods.pdf</t>
+  </si>
+  <si>
+    <t>PartD_Prescriber_PUF_NPI_Drug_13.txt</t>
+  </si>
+  <si>
+    <t>PartD_Prescriber_PUF_NPI_Drug_14.txt</t>
+  </si>
+  <si>
+    <t>PartD_Prescriber_PUF_NPI_Drug_15.txt</t>
+  </si>
+  <si>
+    <t>PartD_Prescriber_PUF_NPI_Drug_16.txt</t>
+  </si>
+  <si>
+    <t>PartD_Prescriber_PUF_NPI_Drug_17.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prescriber methods/codebook </t>
+  </si>
+  <si>
+    <t>zipcodes_nt/</t>
+  </si>
+  <si>
+    <t>Folder with MA postal zipcode shapefiles</t>
+  </si>
+  <si>
+    <t>Used to merge opioid prescribers with MA opioid overdose death town</t>
+  </si>
+  <si>
+    <t>https://docs.digital.mass.gov/dataset/massgis-data-zip-codes-5-digit-here-navteq-0</t>
+  </si>
+  <si>
+    <t>ma_town_crs4326_coords.csv</t>
+  </si>
+  <si>
+    <t>Lat/Lon for centroid associated with 351 MA municipalities</t>
+  </si>
+  <si>
+    <t>Modeling</t>
+  </si>
+  <si>
+    <t>notebook_3_ma_census_block_and_town_match.ipynb</t>
+  </si>
+  <si>
+    <t>Shapefile of 351 MA municipalities</t>
+  </si>
+  <si>
+    <t>Modeling - used to account for geospatial component in data</t>
+  </si>
+  <si>
+    <t>ma_total_overdose_for_graph.csv</t>
+  </si>
+  <si>
+    <t>Used to create plot of total opioid overdose deaths by year in MA</t>
+  </si>
+  <si>
+    <t>Total opioid overdose death counts per year (years 2000-2018)</t>
+  </si>
+  <si>
+    <t>Numbers copid from Figure 2 in the Data Brief: Opioid-Related OverdoseDeaths among Massachusetts Residents pdf</t>
+  </si>
+  <si>
+    <t>500_cities_totpop_metric_pivot_table.csv</t>
+  </si>
+  <si>
+    <t>Part of the 500 city health dashboard dataset</t>
+  </si>
+  <si>
+    <t>notebook_1_city_health_dash_500_cities_opioid_corr.ipynb</t>
+  </si>
+  <si>
+    <t>500 cities dataset &gt; selected general population only, at the city level - metrics relating to city health, including opioid overdose deaths</t>
+  </si>
+  <si>
+    <t>Used to create the opioid overdose death correlation figure (500 cities dataset)</t>
+  </si>
+  <si>
+    <t>census_block_town_match.csv</t>
+  </si>
+  <si>
+    <t>Town - census block GEOID (2010) associations</t>
+  </si>
+  <si>
+    <t>Created from the centroid spatial join of 2010 census block shapefile and the MA 351 municipality shapefile</t>
+  </si>
+  <si>
+    <t>Used to join and summarize the 2017 ACS dataset to the 351 MA opioid overdose death municipalities</t>
+  </si>
+  <si>
+    <t>census_block_town_match_2010pop_error.csv</t>
+  </si>
+  <si>
+    <t>Same as the census_block_town_match file, but includes the 2010 expected vs estimated population and errors</t>
+  </si>
+  <si>
+    <t>Used to understand the error in the census block / town merge</t>
+  </si>
+  <si>
+    <t>overdose_death_count_acs_merge.csv</t>
+  </si>
+  <si>
+    <t>notebook_4_overdose_death_and_acs_by_census_block_merge_and_eda.ipynb</t>
+  </si>
+  <si>
+    <t>Wide format of MA opioid overdose death count merge and 2017 ACS data merge, using the census block - town match dataset</t>
+  </si>
+  <si>
+    <t>Merge of ma_town_opioid_overdose_death_by_place_of_death_2014_to_2018.csv and R12288202_SL150.csv (2017 ACS data); Population estimates derived from an assumption of a linear change per year from 2010 to 2017</t>
+  </si>
+  <si>
+    <t>Modeling, later futher merged with opioid claims data</t>
+  </si>
+  <si>
+    <t>medicare_partD_opioid_prescriber_2013_w_zip_MAtown_v1.csv</t>
+  </si>
+  <si>
+    <t>medicare_partD_opioid_prescriber_2014_w_zip_MAtown_v1.csv</t>
+  </si>
+  <si>
+    <t>medicare_partD_opioid_prescriber_2015_w_zip_MAtown_v1.csv</t>
+  </si>
+  <si>
+    <t>medicare_partD_opioid_prescriber_2016_w_zip_MAtown_v1.csv</t>
+  </si>
+  <si>
+    <t>medicare_partD_opioid_prescriber_2017_w_zip_MAtown_v1.csv</t>
+  </si>
+  <si>
+    <t>Medicare opioid prescription dataset, with individual prescribers associated with one of the 351 towns in the MA opioid overdose dataset</t>
+  </si>
+  <si>
+    <t>notebook_5_medicare_opioid_and_nonopioid_prescriber_cleanup_and_town_join.ipynb</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>Raw files in the medicare_prescription_opioids folder, merged with town using the shapefile in the zipcodes_nt folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opioid prescription data per town </t>
+  </si>
+  <si>
+    <t>These datasets have duplicate entries for some prescribers if the zipcode was associated with more than one town in the shapefile. This is resolved in notebook 6 by randomly choosing a town to associate the prescriber with per year</t>
+  </si>
+  <si>
+    <t>medicare_partD_opioid_prescriber_all_years_no_ziptown_duplicates</t>
+  </si>
+  <si>
+    <t>Individual prescribers with no duplicates per year; All years in one file (long format)</t>
+  </si>
+  <si>
+    <t>notebook_6_ma_opioid_overdose_death_and_acs_and_partD_drug_match_by_town.ipynb</t>
+  </si>
+  <si>
+    <t>Modeling, also used to associate Benzodiazepine prescribers with a town based on NPI code</t>
+  </si>
+  <si>
+    <t>5 files above merged into one, with multiple town associations removed</t>
+  </si>
+  <si>
+    <t>final_model_df_with_features_and_pred.csv</t>
+  </si>
+  <si>
+    <t>Final dataset used for modeling, also includes predicted death counts for about 280 towns for all years</t>
+  </si>
+  <si>
+    <t>gam_modeling.rmd (notebook 7)</t>
+  </si>
+  <si>
+    <t>Combination of MA opioid overdose deaths, ACS data, Medicare prescriber opioid data, and Medicare benzodiazepine prescriptions (Medicare prescriber summarized by town)</t>
+  </si>
+  <si>
+    <t>Reference, figure generation</t>
+  </si>
+  <si>
+    <t>med_partD_benzo_indiv_pres_w_town_merge_13_to_17.csv</t>
+  </si>
+  <si>
+    <t>Individual benzodiazepine prescribers, associated with a  town, all 3 benzodiazepines of interest represented</t>
+  </si>
+  <si>
+    <t>Came from the large all-drug medicare utilization files, town association through the opioid prescribers by NPI (from the no duplicate file)</t>
+  </si>
+  <si>
+    <t>Original dataset did include a town, but the town names did not match well with the 351 town in the opioid overdose death dataset - there were too many</t>
+  </si>
+  <si>
+    <t>med_partD_benzo_sum_w_town_merge_13_to_17.csv</t>
+  </si>
+  <si>
+    <t>Benzodiazepine prescriptions, claims summarized by town</t>
+  </si>
+  <si>
+    <t>Dataset above, summarized by town</t>
+  </si>
+  <si>
+    <t>This dataset was the main reason why the town count went down from 351 -&gt; ~280</t>
   </si>
 </sst>
 </file>
@@ -716,87 +919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891DE753-94C5-49D5-A840-92C5F085CC82}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346E222B-442B-4376-8D3F-E3761B1F991A}">
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="45.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346E222B-442B-4376-8D3F-E3761B1F991A}">
-  <dimension ref="A1:G49"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,7 +935,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -816,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -825,112 +952,112 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
         <v>43723</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1">
         <v>43723</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
         <v>43723</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1">
         <v>43723</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1">
         <v>43723</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -938,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -947,58 +1074,58 @@
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1">
         <v>43721</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1">
         <v>43721</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1006,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
@@ -1015,97 +1142,97 @@
         <v>2</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E18" s="1">
         <v>43720</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E19" s="1">
         <v>43723</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1">
         <v>43723</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E21" s="1">
         <v>43723</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1113,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>1</v>
@@ -1122,170 +1249,241 @@
         <v>2</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="1">
+        <v>43733</v>
+      </c>
+      <c r="F28" t="s">
+        <v>104</v>
+      </c>
+      <c r="G28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="1">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="1">
+        <v>43733</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>84</v>
+      <c r="A31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="1">
+        <v>43730</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>30</v>
+      <c r="A32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="1">
+        <v>43725</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="1">
-        <v>43719</v>
-      </c>
-      <c r="F33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="1">
-        <v>43719</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="1">
-        <v>43719</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="1">
-        <v>43719</v>
+      <c r="A36" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="1">
-        <v>43719</v>
+      <c r="A37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="1">
+        <v>43719</v>
+      </c>
+      <c r="F38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="1">
+        <v>43719</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
-        <v>93</v>
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="1">
+        <v>43719</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>30</v>
+      <c r="E42" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1293,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>1</v>
@@ -1302,76 +1500,124 @@
         <v>2</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" t="s">
-        <v>99</v>
-      </c>
-      <c r="E48" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="1">
         <v>43723</v>
       </c>
-      <c r="F48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" s="1">
+      <c r="F53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="1">
         <v>43724</v>
       </c>
-      <c r="F49" t="s">
-        <v>102</v>
+      <c r="F54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E55" s="1">
+        <v>43724</v>
+      </c>
+      <c r="F55" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{A06239DA-1EF7-48F0-8B85-18B252279A34}"/>
     <hyperlink ref="D18" r:id="rId2" xr:uid="{57B83395-7527-4B74-A1DA-E565991406F3}"/>
-    <hyperlink ref="D33" r:id="rId3" xr:uid="{2958F1B8-0368-4195-8497-5925E3429781}"/>
-    <hyperlink ref="D34" r:id="rId4" xr:uid="{8BD99E14-70C7-4D70-A35F-8785C13C4DFA}"/>
-    <hyperlink ref="D35" r:id="rId5" xr:uid="{DF933CB7-EB9F-4605-A6F1-4340BAB67BCD}"/>
-    <hyperlink ref="D36" r:id="rId6" xr:uid="{6B7D5CBE-6D80-43E9-8D1F-F409047BFB63}"/>
-    <hyperlink ref="D37" r:id="rId7" xr:uid="{795FA866-B3AE-49B1-B806-F6A0B9BFE0D8}"/>
+    <hyperlink ref="D38" r:id="rId3" xr:uid="{2958F1B8-0368-4195-8497-5925E3429781}"/>
+    <hyperlink ref="D39" r:id="rId4" xr:uid="{8BD99E14-70C7-4D70-A35F-8785C13C4DFA}"/>
+    <hyperlink ref="D40" r:id="rId5" xr:uid="{DF933CB7-EB9F-4605-A6F1-4340BAB67BCD}"/>
+    <hyperlink ref="D41" r:id="rId6" xr:uid="{6B7D5CBE-6D80-43E9-8D1F-F409047BFB63}"/>
+    <hyperlink ref="D42" r:id="rId7" xr:uid="{795FA866-B3AE-49B1-B806-F6A0B9BFE0D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64ADABC0-9B8B-44DE-B09A-F3870EA4FA63}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1384,7 +1630,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1392,56 +1638,317 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>